<commit_message>
All odal can open
</commit_message>
<xml_diff>
--- a/AI_commands.xlsx
+++ b/AI_commands.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>VUE.js keretrendszerben formázni kell úgy a beviteli mezőket tartalmazó kódrészletet, hogy az oldal közepére kerüljön és vízszintes 1024 képpontig az oldal 33 százalékát töltse ki. Az alatt az oldalszélesség 80 százalékát.</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>VUE.js programból a modális rész legyen áthelyezve egy ModalNew.vue komponensbe és a TaskItem.vue hívja meg.</t>
+  </si>
+  <si>
+    <t>VUE.js program: Hogyan tudnám a CloseFun() funkcióban az isVisible értéket falsra állítani és így bezárni az ablakot?</t>
   </si>
 </sst>
 </file>
@@ -417,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B22"/>
+  <dimension ref="A2:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +590,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Token protection has been added
</commit_message>
<xml_diff>
--- a/AI_commands.xlsx
+++ b/AI_commands.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>VUE.js keretrendszerben formázni kell úgy a beviteli mezőket tartalmazó kódrészletet, hogy az oldal közepére kerüljön és vízszintes 1024 képpontig az oldal 33 százalékát töltse ki. Az alatt az oldalszélesség 80 százalékát.</t>
   </si>
@@ -94,6 +94,33 @@
   </si>
   <si>
     <t xml:space="preserve"> VUE.js program: Adatkérés után hogyan frissítsem az oldalt, hogy megjelenjen a legfrissebb állapot?</t>
+  </si>
+  <si>
+    <t>Milyen telepíthető auth-token lehetőségek vannak?</t>
+  </si>
+  <si>
+    <t>Hogyan adok hozzá Django REST framework TokenAuthentication-t a meglévő programhoz?</t>
+  </si>
+  <si>
+    <t>Django-REST-Knox van telepítve. Kérem a view.py és az url.py részeinek megírását,  az API-n keresztül  regisztrálás, login és logout működjöm.</t>
+  </si>
+  <si>
+    <t>Az előző megoldás esetén a  jelszó olvasható módon került tárolásra regisztráláskor nem lett HASH-elve, mit kell változtatni?</t>
+  </si>
+  <si>
+    <t>Írd át a LoginView és a LogoutView részeket, hogy a HASH jelszavakat kezelje:</t>
+  </si>
+  <si>
+    <t>Mit  kell megadni az előzőekben létrehozottban a sikeres logaout-hoz?</t>
+  </si>
+  <si>
+    <t>Milyen adatokat kell megadni az API POST kéréshez?</t>
+  </si>
+  <si>
+    <t>Alakítsd át úgy, hogy kártya "card" formában legyen a bejelentkezés form. Kékből zöldbe bal felső sarokból jobba színátmenetes háttérrel:</t>
+  </si>
+  <si>
+    <t>Ez alőzőben létrehozott kártya az input mezők szélességéhez képest 20%-al legyen nagyobb!</t>
   </si>
 </sst>
 </file>
@@ -423,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B24"/>
+  <dimension ref="A2:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,28 +606,109 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logout function has been added
</commit_message>
<xml_diff>
--- a/AI_commands.xlsx
+++ b/AI_commands.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>VUE.js keretrendszerben formázni kell úgy a beviteli mezőket tartalmazó kódrészletet, hogy az oldal közepére kerüljön és vízszintes 1024 képpontig az oldal 33 százalékát töltse ki. Az alatt az oldalszélesség 80 százalékát.</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t xml:space="preserve">VUE.js &lt;templatben&gt;, hogyan adjam meg változóval, hogy egy link aktív vagy nem az </t>
+  </si>
+  <si>
+    <t>Hogyan kell kitörölni a böngéső localStorage tartalmát JavaScript használatával</t>
+  </si>
+  <si>
+    <t>Hogyan kell beletenni a tokent az alábbi hívásba? (Fejrészben [{"key":"Authorization","value":"Token eeb1dca2fb50531e82cb8433aa458d3d3d8abc52b8c235d98ca561a90b192662","type":"text","enabled":false}]</t>
+  </si>
+  <si>
+    <t>Hogyan kell a főoldalt betölteni és friisíteni is? (A navbár különben nem frissül)</t>
   </si>
 </sst>
 </file>
@@ -173,11 +182,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -194,6 +206,95 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1025" name="AutoShape 1" descr="data:image/svg+xml,%3csvg%20xmlns=%27http://www.w3.org/2000/svg%27%20version=%271.1%27%20width=%2738%27%20height=%2738%27/%3e"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="7562850"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1026" name="AutoShape 2" descr="User"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="7562850"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B36"/>
+  <dimension ref="A2:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,17 +836,78 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
       <c r="B36" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cardset checked REST with token
</commit_message>
<xml_diff>
--- a/AI_commands.xlsx
+++ b/AI_commands.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>VUE.js keretrendszerben formázni kell úgy a beviteli mezőket tartalmazó kódrészletet, hogy az oldal közepére kerüljön és vízszintes 1024 képpontig az oldal 33 százalékát töltse ki. Az alatt az oldalszélesség 80 százalékát.</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>Hogyan kell a főoldalt betölteni és friisíteni is? (A navbár különben nem frissül)</t>
+  </si>
+  <si>
+    <t>Hogyan kell hozzáadni a REST-KNOX token autorizációt?</t>
+  </si>
+  <si>
+    <t>A @authentication_classes dekorátorhoz mit kell importálni?</t>
   </si>
 </sst>
 </file>
@@ -275,6 +281,90 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="923925" y="7562850"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 1" descr="data:image/svg+xml,%3csvg%20xmlns=%27http://www.w3.org/2000/svg%27%20version=%271.1%27%20width=%2738%27%20height=%2738%27/%3e"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8382000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2" descr="User"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="923925" y="8382000"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -563,7 +653,7 @@
   <dimension ref="A2:B45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,14 +965,20 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>